<commit_message>
add view from 1 -> 5
</commit_message>
<xml_diff>
--- a/Resources/Sheet/Book1.xlsx
+++ b/Resources/Sheet/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\document\Thaiha\BoDoiApp\Resources\Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89943E5C-105E-4B71-B294-9E074A2ED9E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353F6F7E-9138-49E2-B98E-0D47C34098F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{FCE59EA9-790B-433B-B511-234C9C16BD72}"/>
   </bookViews>
@@ -552,6 +552,15 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -576,6 +585,9 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -589,18 +601,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -926,76 +926,76 @@
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="24"/>
+      <c r="A1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="27"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="27"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="30"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28" t="s">
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28" t="s">
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
       <c r="L4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1004,8 +1004,8 @@
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="31"/>
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1021,7 +1021,7 @@
       <c r="G5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="28"/>
+      <c r="H5" s="31"/>
       <c r="I5" s="1">
         <v>60</v>
       </c>
@@ -1360,76 +1360,76 @@
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="24"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="27"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="27"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="30"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28" t="s">
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28" t="s">
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
       <c r="L4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1438,8 +1438,8 @@
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="31"/>
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1455,7 +1455,7 @@
       <c r="G5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="28"/>
+      <c r="H5" s="31"/>
       <c r="I5" s="1">
         <v>60</v>
       </c>
@@ -1935,201 +1935,211 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="33" t="s">
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="37" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="35" t="s">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="38">
+      <c r="C3" s="23">
+        <v>36</v>
+      </c>
+      <c r="D3" s="24">
         <v>35</v>
       </c>
-      <c r="E3" s="37" t="e">
+      <c r="E3" s="23">
         <f>D3/C3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F3" s="37">
+        <v>0.97222222222222221</v>
+      </c>
+      <c r="F3" s="23">
         <f>G3/D3</f>
         <v>0.97142857142857142</v>
       </c>
-      <c r="G3" s="38">
+      <c r="G3" s="24">
         <v>34</v>
       </c>
-      <c r="H3" s="38"/>
-      <c r="I3" s="37">
+      <c r="H3" s="24"/>
+      <c r="I3" s="23">
         <f>C3-D3</f>
-        <v>-35</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="38">
+      <c r="C4" s="23">
         <v>439</v>
       </c>
-      <c r="E4" s="37" t="e">
+      <c r="D4" s="24">
+        <v>439</v>
+      </c>
+      <c r="E4" s="23">
         <f>D4/C4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F4" s="37">
+        <v>1</v>
+      </c>
+      <c r="F4" s="23">
         <f t="shared" ref="F4:F7" si="0">G4/D4</f>
         <v>0.99772209567198178</v>
       </c>
-      <c r="G4" s="38">
+      <c r="G4" s="24">
         <v>438</v>
       </c>
-      <c r="H4" s="38"/>
-      <c r="I4" s="37">
+      <c r="H4" s="24"/>
+      <c r="I4" s="23">
         <f>C4-D4</f>
-        <v>-439</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="38">
+      <c r="C5" s="23">
         <v>27</v>
       </c>
-      <c r="E5" s="37" t="e">
+      <c r="D5" s="24">
+        <v>27</v>
+      </c>
+      <c r="E5" s="23">
         <f>D5/C5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F5" s="37">
+        <v>1</v>
+      </c>
+      <c r="F5" s="23">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G5" s="38">
+      <c r="G5" s="24">
         <v>27</v>
       </c>
-      <c r="H5" s="38"/>
-      <c r="I5" s="37">
-        <f t="shared" ref="I4:I7" si="1">C5-D5</f>
-        <v>-27</v>
+      <c r="H5" s="24"/>
+      <c r="I5" s="23">
+        <f t="shared" ref="I5:I7" si="1">C5-D5</f>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="37"/>
-      <c r="D6" s="38">
+      <c r="C6" s="23">
         <v>6</v>
       </c>
-      <c r="E6" s="37" t="e">
+      <c r="D6" s="24">
+        <v>6</v>
+      </c>
+      <c r="E6" s="23">
         <f>D6/C6</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F6" s="37">
+        <v>1</v>
+      </c>
+      <c r="F6" s="23">
         <f t="shared" si="0"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="G6" s="38">
+      <c r="G6" s="24">
         <v>5</v>
       </c>
-      <c r="H6" s="38"/>
-      <c r="I6" s="37">
-        <f t="shared" si="1"/>
-        <v>-6</v>
+      <c r="H6" s="24"/>
+      <c r="I6" s="23">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="38">
+      <c r="C7" s="23">
         <v>2073</v>
       </c>
-      <c r="E7" s="37" t="e">
+      <c r="D7" s="24">
+        <v>2073</v>
+      </c>
+      <c r="E7" s="23">
         <f>D7/C7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F7" s="37">
+        <v>1</v>
+      </c>
+      <c r="F7" s="23">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G7" s="38">
+      <c r="G7" s="24">
         <v>2073</v>
       </c>
-      <c r="H7" s="38"/>
-      <c r="I7" s="37">
-        <f t="shared" si="1"/>
-        <v>-2073</v>
+      <c r="H7" s="24"/>
+      <c r="I7" s="23">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="I1:I2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
sửa header cho các form
</commit_message>
<xml_diff>
--- a/Resources/Sheet/Book1.xlsx
+++ b/Resources/Sheet/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\document\Thaiha\BoDoiApp\Resources\Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC471223-8ACC-4267-B413-FB9B8E6FD216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68EA380-13DD-4777-92DD-DC4E4894C1FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="5" xr2:uid="{FCE59EA9-790B-433B-B511-234C9C16BD72}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="7" xr2:uid="{FCE59EA9-790B-433B-B511-234C9C16BD72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="115">
   <si>
     <t>TỔ CHỨC BIÊN CHẾ, TRANG BỊ HƯỚNG CHỦ YẾU</t>
   </si>
@@ -231,13 +233,183 @@
   </si>
   <si>
     <t>Đơn vị</t>
+  </si>
+  <si>
+    <t>Nội dung</t>
+  </si>
+  <si>
+    <t>Quân số</t>
+  </si>
+  <si>
+    <t>Vũ khí trang bị kỹ thuật</t>
+  </si>
+  <si>
+    <t>Phân chia lực lượng</t>
+  </si>
+  <si>
+    <t>SQ</t>
+  </si>
+  <si>
+    <t>QNCN</t>
+  </si>
+  <si>
+    <t>HSQ-BS</t>
+  </si>
+  <si>
+    <t>Vũ khí</t>
+  </si>
+  <si>
+    <t>Xe-máy</t>
+  </si>
+  <si>
+    <t>TB khác</t>
+  </si>
+  <si>
+    <t>Bộ phận HC-KT</t>
+  </si>
+  <si>
+    <t>Lực lượng tăng cường cho đơn vị</t>
+  </si>
+  <si>
+    <t>QS</t>
+  </si>
+  <si>
+    <t>TB</t>
+  </si>
+  <si>
+    <t>Tên TBKT</t>
+  </si>
+  <si>
+    <t>Đơn vị tính</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nhu cầu </t>
+  </si>
+  <si>
+    <t>Phải có trước CĐ</t>
+  </si>
+  <si>
+    <t>Phải bổ sung</t>
+  </si>
+  <si>
+    <t>Tổng số</t>
+  </si>
+  <si>
+    <r>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>bđ</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>t</t>
+    </r>
+  </si>
+  <si>
+    <t>Số lượng</t>
+  </si>
+  <si>
+    <t>Thời gian</t>
+  </si>
+  <si>
+    <t>Địa điểm</t>
+  </si>
+  <si>
+    <t>Phương thức</t>
+  </si>
+  <si>
+    <t>dBB1+PT</t>
+  </si>
+  <si>
+    <t>SMPK 12,7mm</t>
+  </si>
+  <si>
+    <t>Cối 100mm/e</t>
+  </si>
+  <si>
+    <t>Cối 82mm/d</t>
+  </si>
+  <si>
+    <t>Cối 60mm</t>
+  </si>
+  <si>
+    <t>Súng SPG-9</t>
+  </si>
+  <si>
+    <t>Súng B41</t>
+  </si>
+  <si>
+    <t>Súng đại liên</t>
+  </si>
+  <si>
+    <t>Súng trung liên</t>
+  </si>
+  <si>
+    <t>Súng tiểu liên</t>
+  </si>
+  <si>
+    <t>Súng ngắn</t>
+  </si>
+  <si>
+    <t>quả</t>
+  </si>
+  <si>
+    <t>Hướng PN chủ yếu</t>
+  </si>
+  <si>
+    <t>Cối 82mm</t>
+  </si>
+  <si>
+    <t>Hướng PN thứ yếu</t>
+  </si>
+  <si>
+    <t>Hướng PN phía sau</t>
+  </si>
+  <si>
+    <t>Lực lượng còn lại</t>
+  </si>
+  <si>
+    <t>Cối 100mm</t>
+  </si>
+  <si>
+    <t>14.00 N-4</t>
+  </si>
+  <si>
+    <t>VTCH/đv</t>
+  </si>
+  <si>
+    <t>Tay ba</t>
+  </si>
+  <si>
+    <t>  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -347,8 +519,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="subscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -391,8 +591,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -540,11 +746,96 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -630,6 +921,39 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="18" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -702,22 +1026,37 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="18" fillId="8" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1043,76 +1382,76 @@
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="31"/>
+      <c r="A1" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="42"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="32"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="34"/>
+      <c r="A2" s="43"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="45"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="35" t="s">
+      <c r="A3" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="35"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35" t="s">
+      <c r="A4" s="46"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35" t="s">
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="35" t="s">
+      <c r="I4" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
       <c r="L4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1121,8 +1460,8 @@
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="35"/>
-      <c r="B5" s="35"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="46"/>
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1138,7 +1477,7 @@
       <c r="G5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="35"/>
+      <c r="H5" s="46"/>
       <c r="I5" s="1">
         <v>60</v>
       </c>
@@ -1477,76 +1816,76 @@
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="31"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="42"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="32"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="34"/>
+      <c r="A2" s="43"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="45"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="35" t="s">
+      <c r="A3" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="35"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35" t="s">
+      <c r="A4" s="46"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35" t="s">
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="35" t="s">
+      <c r="I4" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
       <c r="L4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1555,8 +1894,8 @@
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="35"/>
-      <c r="B5" s="35"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="46"/>
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1572,7 +1911,7 @@
       <c r="G5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="35"/>
+      <c r="H5" s="46"/>
       <c r="I5" s="1">
         <v>60</v>
       </c>
@@ -2058,32 +2397,32 @@
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="36" t="s">
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="47" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="39"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
+      <c r="A2" s="50"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
       <c r="D2" s="22" t="s">
         <v>46</v>
       </c>
@@ -2096,8 +2435,8 @@
       <c r="G2" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="23" t="s">
@@ -2371,30 +2710,30 @@
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="48"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="50" t="s">
+      <c r="E1" s="59"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="51"/>
-      <c r="I1" s="52"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="63"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="44"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
+      <c r="A2" s="55"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
       <c r="D2" s="26" t="s">
         <v>65</v>
       </c>
@@ -2495,83 +2834,83 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A90BB609-02C3-4480-ABA1-81B8EB7FC6E5}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection sqref="A1:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="55"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="42"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="56"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="58"/>
+      <c r="A2" s="43"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="45"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="35" t="s">
+      <c r="A3" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="35"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35" t="s">
+      <c r="A4" s="46"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35" t="s">
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="35" t="s">
+      <c r="I4" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
       <c r="L4" s="1" t="s">
         <v>7</v>
       </c>
@@ -2580,8 +2919,8 @@
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="35"/>
-      <c r="B5" s="35"/>
+      <c r="A5" s="46"/>
+      <c r="B5" s="46"/>
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
@@ -2597,7 +2936,7 @@
       <c r="G5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="35"/>
+      <c r="H5" s="46"/>
       <c r="I5" s="1">
         <v>60</v>
       </c>
@@ -3070,4 +3409,1931 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18CCF06B-A044-4E5A-A947-A016657D51E8}">
+  <dimension ref="A1:M4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="64" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="64" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="64"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="64"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="64" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="64" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="64" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="64" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="64" t="s">
+        <v>75</v>
+      </c>
+      <c r="I2" s="64" t="s">
+        <v>76</v>
+      </c>
+      <c r="J2" s="64" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2" s="64"/>
+      <c r="L2" s="65" t="s">
+        <v>78</v>
+      </c>
+      <c r="M2" s="65"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="64"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="65"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="64"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="K4" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="L4" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="M4" s="29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="J2:K3"/>
+    <mergeCell ref="L2:M3"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B9BFD24-F416-4E13-BF3D-CA2831AC61D2}">
+  <dimension ref="A1:M47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="7" max="7" width="4.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="15.5" customHeight="1" thickBot="1">
+      <c r="A1" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="72" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="72" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="72" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="66" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="72" t="s">
+        <v>84</v>
+      </c>
+      <c r="J1" s="66" t="s">
+        <v>85</v>
+      </c>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="68"/>
+    </row>
+    <row r="2" spans="1:13" ht="30.5" thickBot="1">
+      <c r="A2" s="73"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2" s="73"/>
+      <c r="J2" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="K2" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="L2" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="M2" s="30" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="18.5" customHeight="1" thickBot="1">
+      <c r="A3" s="69" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="33">
+        <v>9</v>
+      </c>
+      <c r="E3" s="33">
+        <v>9</v>
+      </c>
+      <c r="F3" s="33">
+        <v>9</v>
+      </c>
+      <c r="G3" s="33">
+        <f>E3/D3</f>
+        <v>1</v>
+      </c>
+      <c r="H3" s="33">
+        <f>F3/E3</f>
+        <v>1</v>
+      </c>
+      <c r="I3" s="33">
+        <f>D3</f>
+        <v>9</v>
+      </c>
+      <c r="J3" s="33">
+        <f>D3-E3</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+    </row>
+    <row r="4" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A4" s="70"/>
+      <c r="B4" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="35">
+        <v>4</v>
+      </c>
+      <c r="E4" s="33">
+        <v>4</v>
+      </c>
+      <c r="F4" s="33">
+        <v>4</v>
+      </c>
+      <c r="G4" s="33">
+        <f t="shared" ref="G4:H47" si="0">E4/D4</f>
+        <v>1</v>
+      </c>
+      <c r="H4" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I4" s="33">
+        <f t="shared" ref="I4:I47" si="1">D4</f>
+        <v>4</v>
+      </c>
+      <c r="J4" s="33">
+        <f t="shared" ref="J4:J47" si="2">D4-E4</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+    </row>
+    <row r="5" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A5" s="70"/>
+      <c r="B5" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="35">
+        <v>4</v>
+      </c>
+      <c r="E5" s="33">
+        <v>4</v>
+      </c>
+      <c r="F5" s="33">
+        <v>4</v>
+      </c>
+      <c r="G5" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H5" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I5" s="33">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J5" s="33">
+        <f>D5-E5</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+    </row>
+    <row r="6" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A6" s="70"/>
+      <c r="B6" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="35">
+        <v>8</v>
+      </c>
+      <c r="E6" s="33">
+        <v>8</v>
+      </c>
+      <c r="F6" s="33">
+        <v>8</v>
+      </c>
+      <c r="G6" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H6" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I6" s="33">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J6" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+    </row>
+    <row r="7" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A7" s="70"/>
+      <c r="B7" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="35">
+        <v>9</v>
+      </c>
+      <c r="E7" s="33">
+        <v>9</v>
+      </c>
+      <c r="F7" s="33">
+        <v>9</v>
+      </c>
+      <c r="G7" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H7" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I7" s="33">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="J7" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+    </row>
+    <row r="8" spans="1:13" ht="36.5" thickBot="1">
+      <c r="A8" s="70"/>
+      <c r="B8" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="35">
+        <v>72</v>
+      </c>
+      <c r="E8" s="33">
+        <v>72</v>
+      </c>
+      <c r="F8" s="33">
+        <v>71</v>
+      </c>
+      <c r="G8" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H8" s="36">
+        <f t="shared" si="0"/>
+        <v>0.98611111111111116</v>
+      </c>
+      <c r="I8" s="33">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="J8" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="L8" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="M8" s="31" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A9" s="70"/>
+      <c r="B9" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="35">
+        <v>8</v>
+      </c>
+      <c r="E9" s="33">
+        <v>8</v>
+      </c>
+      <c r="F9" s="33">
+        <v>8</v>
+      </c>
+      <c r="G9" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H9" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I9" s="33">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J9" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+    </row>
+    <row r="10" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A10" s="70"/>
+      <c r="B10" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="35">
+        <v>36</v>
+      </c>
+      <c r="E10" s="33">
+        <v>36</v>
+      </c>
+      <c r="F10" s="33">
+        <v>36</v>
+      </c>
+      <c r="G10" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H10" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I10" s="33">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="J10" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+    </row>
+    <row r="11" spans="1:13" ht="36.5" thickBot="1">
+      <c r="A11" s="70"/>
+      <c r="B11" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="35">
+        <v>486</v>
+      </c>
+      <c r="E11" s="33">
+        <v>486</v>
+      </c>
+      <c r="F11" s="33">
+        <v>474</v>
+      </c>
+      <c r="G11" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H11" s="36">
+        <f t="shared" si="0"/>
+        <v>0.97530864197530864</v>
+      </c>
+      <c r="I11" s="33">
+        <f t="shared" si="1"/>
+        <v>486</v>
+      </c>
+      <c r="J11" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="L11" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="M11" s="31" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A12" s="70"/>
+      <c r="B12" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="35">
+        <v>42</v>
+      </c>
+      <c r="E12" s="33">
+        <v>42</v>
+      </c>
+      <c r="F12" s="33">
+        <v>42</v>
+      </c>
+      <c r="G12" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H12" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I12" s="33">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="J12" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+    </row>
+    <row r="13" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A13" s="71"/>
+      <c r="B13" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" s="74">
+        <v>2403</v>
+      </c>
+      <c r="E13" s="37">
+        <v>2403</v>
+      </c>
+      <c r="F13" s="37">
+        <v>2403</v>
+      </c>
+      <c r="G13" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H13" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I13" s="33">
+        <f t="shared" si="1"/>
+        <v>2403</v>
+      </c>
+      <c r="J13" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+    </row>
+    <row r="14" spans="1:13" ht="18.5" customHeight="1" thickBot="1">
+      <c r="A14" s="69" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="33">
+        <v>3</v>
+      </c>
+      <c r="E14" s="33">
+        <v>3</v>
+      </c>
+      <c r="F14" s="33">
+        <v>3</v>
+      </c>
+      <c r="G14" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H14" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I14" s="33">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="J14" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
+    </row>
+    <row r="15" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A15" s="70"/>
+      <c r="B15" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="35">
+        <v>3</v>
+      </c>
+      <c r="E15" s="33">
+        <v>3</v>
+      </c>
+      <c r="F15" s="33">
+        <v>3</v>
+      </c>
+      <c r="G15" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H15" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I15" s="33">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="J15" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+    </row>
+    <row r="16" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A16" s="70"/>
+      <c r="B16" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="35">
+        <v>4</v>
+      </c>
+      <c r="E16" s="33">
+        <v>4</v>
+      </c>
+      <c r="F16" s="33">
+        <v>4</v>
+      </c>
+      <c r="G16" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H16" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I16" s="33">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J16" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="31"/>
+    </row>
+    <row r="17" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A17" s="70"/>
+      <c r="B17" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="35">
+        <v>3</v>
+      </c>
+      <c r="E17" s="33">
+        <v>3</v>
+      </c>
+      <c r="F17" s="33">
+        <v>3</v>
+      </c>
+      <c r="G17" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H17" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I17" s="33">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="J17" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31"/>
+    </row>
+    <row r="18" spans="1:13" ht="36.5" thickBot="1">
+      <c r="A18" s="70"/>
+      <c r="B18" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="35">
+        <v>30</v>
+      </c>
+      <c r="E18" s="33">
+        <v>30</v>
+      </c>
+      <c r="F18" s="33">
+        <v>29</v>
+      </c>
+      <c r="G18" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H18" s="36">
+        <f t="shared" si="0"/>
+        <v>0.96666666666666667</v>
+      </c>
+      <c r="I18" s="33">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="J18" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="L18" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="M18" s="31" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A19" s="70"/>
+      <c r="B19" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="35">
+        <v>4</v>
+      </c>
+      <c r="E19" s="33">
+        <v>4</v>
+      </c>
+      <c r="F19" s="33">
+        <v>4</v>
+      </c>
+      <c r="G19" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H19" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I19" s="33">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J19" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="31"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="31"/>
+    </row>
+    <row r="20" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A20" s="70"/>
+      <c r="B20" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="35">
+        <v>18</v>
+      </c>
+      <c r="E20" s="33">
+        <v>18</v>
+      </c>
+      <c r="F20" s="33">
+        <v>18</v>
+      </c>
+      <c r="G20" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H20" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I20" s="33">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="J20" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="31"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="31"/>
+    </row>
+    <row r="21" spans="1:13" ht="36.5" thickBot="1">
+      <c r="A21" s="70"/>
+      <c r="B21" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="35">
+        <v>161</v>
+      </c>
+      <c r="E21" s="33">
+        <v>161</v>
+      </c>
+      <c r="F21" s="33">
+        <v>155</v>
+      </c>
+      <c r="G21" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H21" s="36">
+        <f t="shared" si="0"/>
+        <v>0.96273291925465843</v>
+      </c>
+      <c r="I21" s="33">
+        <f t="shared" si="1"/>
+        <v>161</v>
+      </c>
+      <c r="J21" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="L21" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="M21" s="31" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A22" s="70"/>
+      <c r="B22" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="35">
+        <v>12</v>
+      </c>
+      <c r="E22" s="33">
+        <v>12</v>
+      </c>
+      <c r="F22" s="33">
+        <v>12</v>
+      </c>
+      <c r="G22" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H22" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I22" s="33">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="J22" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K22" s="31"/>
+      <c r="L22" s="31"/>
+      <c r="M22" s="31"/>
+    </row>
+    <row r="23" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A23" s="71"/>
+      <c r="B23" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="35">
+        <v>846</v>
+      </c>
+      <c r="E23" s="33">
+        <v>846</v>
+      </c>
+      <c r="F23" s="33">
+        <v>846</v>
+      </c>
+      <c r="G23" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H23" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I23" s="33">
+        <f t="shared" si="1"/>
+        <v>846</v>
+      </c>
+      <c r="J23" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="31"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="31"/>
+    </row>
+    <row r="24" spans="1:13" ht="18.5" customHeight="1" thickBot="1">
+      <c r="A24" s="69" t="s">
+        <v>107</v>
+      </c>
+      <c r="B24" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="33">
+        <v>3</v>
+      </c>
+      <c r="E24" s="33">
+        <v>3</v>
+      </c>
+      <c r="F24" s="33">
+        <v>3</v>
+      </c>
+      <c r="G24" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H24" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I24" s="33">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="J24" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
+    </row>
+    <row r="25" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A25" s="70"/>
+      <c r="B25" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="33">
+        <v>1</v>
+      </c>
+      <c r="E25" s="33">
+        <v>1</v>
+      </c>
+      <c r="F25" s="33">
+        <v>1</v>
+      </c>
+      <c r="G25" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H25" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I25" s="33">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J25" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="31"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="31"/>
+    </row>
+    <row r="26" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A26" s="70"/>
+      <c r="B26" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="35">
+        <v>2</v>
+      </c>
+      <c r="E26" s="33">
+        <v>2</v>
+      </c>
+      <c r="F26" s="33">
+        <v>2</v>
+      </c>
+      <c r="G26" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H26" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I26" s="33">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J26" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K26" s="31"/>
+      <c r="L26" s="31"/>
+      <c r="M26" s="31"/>
+    </row>
+    <row r="27" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A27" s="70"/>
+      <c r="B27" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="35">
+        <v>3</v>
+      </c>
+      <c r="E27" s="33">
+        <v>3</v>
+      </c>
+      <c r="F27" s="33">
+        <v>3</v>
+      </c>
+      <c r="G27" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H27" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I27" s="33">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="J27" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="31"/>
+      <c r="L27" s="31"/>
+      <c r="M27" s="31"/>
+    </row>
+    <row r="28" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A28" s="70"/>
+      <c r="B28" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="35">
+        <v>18</v>
+      </c>
+      <c r="E28" s="33">
+        <v>18</v>
+      </c>
+      <c r="F28" s="33">
+        <v>18</v>
+      </c>
+      <c r="G28" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H28" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I28" s="33">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="J28" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K28" s="31"/>
+      <c r="L28" s="31"/>
+      <c r="M28" s="31"/>
+    </row>
+    <row r="29" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A29" s="70"/>
+      <c r="B29" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="35">
+        <v>2</v>
+      </c>
+      <c r="E29" s="33">
+        <v>2</v>
+      </c>
+      <c r="F29" s="33">
+        <v>2</v>
+      </c>
+      <c r="G29" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H29" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I29" s="33">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J29" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K29" s="31"/>
+      <c r="L29" s="31"/>
+      <c r="M29" s="31"/>
+    </row>
+    <row r="30" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A30" s="70"/>
+      <c r="B30" s="39" t="s">
+        <v>101</v>
+      </c>
+      <c r="C30" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="35">
+        <v>9</v>
+      </c>
+      <c r="E30" s="33">
+        <v>9</v>
+      </c>
+      <c r="F30" s="33">
+        <v>9</v>
+      </c>
+      <c r="G30" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H30" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I30" s="33">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="J30" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K30" s="31"/>
+      <c r="L30" s="31"/>
+      <c r="M30" s="31"/>
+    </row>
+    <row r="31" spans="1:13" ht="36.5" thickBot="1">
+      <c r="A31" s="70"/>
+      <c r="B31" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="35">
+        <v>96</v>
+      </c>
+      <c r="E31" s="33">
+        <v>96</v>
+      </c>
+      <c r="F31" s="33">
+        <v>92</v>
+      </c>
+      <c r="G31" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H31" s="36">
+        <f t="shared" si="0"/>
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="I31" s="33">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="J31" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K31" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="L31" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="M31" s="31" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A32" s="70"/>
+      <c r="B32" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="C32" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="35">
+        <v>4</v>
+      </c>
+      <c r="E32" s="33">
+        <v>4</v>
+      </c>
+      <c r="F32" s="33">
+        <v>4</v>
+      </c>
+      <c r="G32" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H32" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I32" s="33">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J32" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K32" s="31"/>
+      <c r="L32" s="31"/>
+      <c r="M32" s="31"/>
+    </row>
+    <row r="33" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A33" s="71"/>
+      <c r="B33" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33" s="35">
+        <v>514</v>
+      </c>
+      <c r="E33" s="33">
+        <v>514</v>
+      </c>
+      <c r="F33" s="33">
+        <v>514</v>
+      </c>
+      <c r="G33" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H33" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I33" s="33">
+        <f t="shared" si="1"/>
+        <v>514</v>
+      </c>
+      <c r="J33" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K33" s="31"/>
+      <c r="L33" s="31"/>
+      <c r="M33" s="31"/>
+    </row>
+    <row r="34" spans="1:13" ht="18.5" customHeight="1" thickBot="1">
+      <c r="A34" s="69" t="s">
+        <v>108</v>
+      </c>
+      <c r="B34" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" s="33">
+        <v>2</v>
+      </c>
+      <c r="E34" s="33">
+        <v>2</v>
+      </c>
+      <c r="F34" s="33">
+        <v>2</v>
+      </c>
+      <c r="G34" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H34" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I34" s="33">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J34" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K34" s="31"/>
+      <c r="L34" s="31"/>
+      <c r="M34" s="31"/>
+    </row>
+    <row r="35" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A35" s="70"/>
+      <c r="B35" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" s="35">
+        <v>18</v>
+      </c>
+      <c r="E35" s="33">
+        <v>18</v>
+      </c>
+      <c r="F35" s="33">
+        <v>18</v>
+      </c>
+      <c r="G35" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H35" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I35" s="33">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="J35" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K35" s="31"/>
+      <c r="L35" s="31"/>
+      <c r="M35" s="31"/>
+    </row>
+    <row r="36" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A36" s="70"/>
+      <c r="B36" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="C36" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" s="35">
+        <v>2</v>
+      </c>
+      <c r="E36" s="33">
+        <v>2</v>
+      </c>
+      <c r="F36" s="33">
+        <v>2</v>
+      </c>
+      <c r="G36" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H36" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I36" s="33">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J36" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K36" s="31"/>
+      <c r="L36" s="31"/>
+      <c r="M36" s="31"/>
+    </row>
+    <row r="37" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A37" s="70"/>
+      <c r="B37" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="C37" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" s="35">
+        <v>9</v>
+      </c>
+      <c r="E37" s="33">
+        <v>9</v>
+      </c>
+      <c r="F37" s="33">
+        <v>9</v>
+      </c>
+      <c r="G37" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H37" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I37" s="33">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="J37" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K37" s="31"/>
+      <c r="L37" s="31"/>
+      <c r="M37" s="31"/>
+    </row>
+    <row r="38" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A38" s="70"/>
+      <c r="B38" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="C38" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" s="35">
+        <v>69</v>
+      </c>
+      <c r="E38" s="33">
+        <v>69</v>
+      </c>
+      <c r="F38" s="33">
+        <v>67</v>
+      </c>
+      <c r="G38" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H38" s="36">
+        <f t="shared" si="0"/>
+        <v>0.97101449275362317</v>
+      </c>
+      <c r="I38" s="33">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="J38" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K38" s="31"/>
+      <c r="L38" s="31"/>
+      <c r="M38" s="31"/>
+    </row>
+    <row r="39" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A39" s="70"/>
+      <c r="B39" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D39" s="35">
+        <v>4</v>
+      </c>
+      <c r="E39" s="33">
+        <v>4</v>
+      </c>
+      <c r="F39" s="33">
+        <v>4</v>
+      </c>
+      <c r="G39" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H39" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I39" s="33">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J39" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K39" s="31"/>
+      <c r="L39" s="31"/>
+      <c r="M39" s="31"/>
+    </row>
+    <row r="40" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A40" s="71"/>
+      <c r="B40" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="D40" s="35">
+        <v>350</v>
+      </c>
+      <c r="E40" s="33">
+        <v>350</v>
+      </c>
+      <c r="F40" s="33">
+        <v>350</v>
+      </c>
+      <c r="G40" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H40" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I40" s="33">
+        <f t="shared" si="1"/>
+        <v>350</v>
+      </c>
+      <c r="J40" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K40" s="31"/>
+      <c r="L40" s="31"/>
+      <c r="M40" s="31"/>
+    </row>
+    <row r="41" spans="1:13" ht="18.5" customHeight="1" thickBot="1">
+      <c r="A41" s="69" t="s">
+        <v>109</v>
+      </c>
+      <c r="B41" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D41" s="33">
+        <v>3</v>
+      </c>
+      <c r="E41" s="33">
+        <v>3</v>
+      </c>
+      <c r="F41" s="33">
+        <v>3</v>
+      </c>
+      <c r="G41" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H41" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I41" s="33">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="J41" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K41" s="31"/>
+      <c r="L41" s="31"/>
+      <c r="M41" s="31" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A42" s="70"/>
+      <c r="B42" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="C42" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D42" s="35">
+        <v>4</v>
+      </c>
+      <c r="E42" s="33">
+        <v>4</v>
+      </c>
+      <c r="F42" s="33">
+        <v>4</v>
+      </c>
+      <c r="G42" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H42" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I42" s="33">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J42" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K42" s="31"/>
+      <c r="L42" s="31"/>
+      <c r="M42" s="31"/>
+    </row>
+    <row r="43" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A43" s="70"/>
+      <c r="B43" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="C43" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D43" s="35">
+        <v>3</v>
+      </c>
+      <c r="E43" s="33">
+        <v>3</v>
+      </c>
+      <c r="F43" s="33">
+        <v>3</v>
+      </c>
+      <c r="G43" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H43" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I43" s="33">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="J43" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K43" s="31"/>
+      <c r="L43" s="31"/>
+      <c r="M43" s="31"/>
+    </row>
+    <row r="44" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A44" s="70"/>
+      <c r="B44" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="C44" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D44" s="35">
+        <v>6</v>
+      </c>
+      <c r="E44" s="33">
+        <v>6</v>
+      </c>
+      <c r="F44" s="33">
+        <v>6</v>
+      </c>
+      <c r="G44" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H44" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I44" s="33">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="J44" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K44" s="31"/>
+      <c r="L44" s="31"/>
+      <c r="M44" s="31"/>
+    </row>
+    <row r="45" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A45" s="70"/>
+      <c r="B45" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="C45" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D45" s="35">
+        <v>160</v>
+      </c>
+      <c r="E45" s="33">
+        <v>160</v>
+      </c>
+      <c r="F45" s="33">
+        <v>160</v>
+      </c>
+      <c r="G45" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H45" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I45" s="33">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="J45" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K45" s="31"/>
+      <c r="L45" s="31"/>
+      <c r="M45" s="31"/>
+    </row>
+    <row r="46" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A46" s="70"/>
+      <c r="B46" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="C46" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D46" s="35">
+        <v>22</v>
+      </c>
+      <c r="E46" s="33">
+        <v>22</v>
+      </c>
+      <c r="F46" s="33">
+        <v>22</v>
+      </c>
+      <c r="G46" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H46" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I46" s="33">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="J46" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K46" s="31"/>
+      <c r="L46" s="31"/>
+      <c r="M46" s="31"/>
+    </row>
+    <row r="47" spans="1:13" ht="18.5" thickBot="1">
+      <c r="A47" s="71"/>
+      <c r="B47" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="D47" s="35">
+        <v>693</v>
+      </c>
+      <c r="E47" s="33">
+        <v>693</v>
+      </c>
+      <c r="F47" s="33">
+        <v>693</v>
+      </c>
+      <c r="G47" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H47" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I47" s="33">
+        <f t="shared" si="1"/>
+        <v>693</v>
+      </c>
+      <c r="J47" s="33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K47" s="31"/>
+      <c r="L47" s="31"/>
+      <c r="M47" s="31"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="A3:A13"/>
+    <mergeCell ref="A14:A23"/>
+    <mergeCell ref="A24:A33"/>
+    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="I1:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>